<commit_message>
Regen - now constrained
</commit_message>
<xml_diff>
--- a/docs/gcms/gcms-metadata.xlsx
+++ b/docs/gcms/gcms-metadata.xlsx
@@ -15,12 +15,13 @@
     <sheet name="ms_source list" sheetId="6" r:id="rId6"/>
     <sheet name="polarity list" sheetId="7" r:id="rId7"/>
     <sheet name="ion_mobility list" sheetId="8" r:id="rId8"/>
-    <sheet name="column_length_unit list" sheetId="9" r:id="rId9"/>
-    <sheet name="column_temp_unit list" sheetId="10" r:id="rId10"/>
-    <sheet name="spatial_type list" sheetId="11" r:id="rId11"/>
-    <sheet name="spatial_sampling_type list" sheetId="12" r:id="rId12"/>
-    <sheet name="resolution_x_unit list" sheetId="13" r:id="rId13"/>
-    <sheet name="resolution_y_unit list" sheetId="14" r:id="rId14"/>
+    <sheet name="data_collection_mode list" sheetId="9" r:id="rId9"/>
+    <sheet name="column_length_unit list" sheetId="10" r:id="rId10"/>
+    <sheet name="column_temp_unit list" sheetId="11" r:id="rId11"/>
+    <sheet name="spatial_type list" sheetId="12" r:id="rId12"/>
+    <sheet name="spatial_sampling_type list" sheetId="13" r:id="rId13"/>
+    <sheet name="resolution_x_unit list" sheetId="14" r:id="rId14"/>
+    <sheet name="resolution_y_unit list" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -661,7 +662,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>version</t>
   </si>
@@ -790,6 +791,12 @@
   </si>
   <si>
     <t>data_collection_mode</t>
+  </si>
+  <si>
+    <t>DDA</t>
+  </si>
+  <si>
+    <t>DIA</t>
   </si>
   <si>
     <t>ms_scan_mode</t>
@@ -1320,80 +1327,80 @@
         <v>42</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="AT1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="22">
+  <dataValidations count="23">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -1433,6 +1440,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: TIMS / TWIMS / FAIMS / DTIMS / SLIMS." sqref="W2:W1048576">
       <formula1>'ion_mobility list'!$A$1:$A$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: DDA / DIA." sqref="X2:X1048576">
+      <formula1>'data_collection_mode list'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AD2:AD1048576">
       <formula1>-1e+307</formula1>
@@ -1484,7 +1494,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1493,6 +1503,24 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -1502,45 +1530,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1558,12 +1563,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1581,12 +1586,35 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1782,7 +1810,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1790,7 +1818,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>